<commit_message>
cleaned up main + updated structure
</commit_message>
<xml_diff>
--- a/Soutenance/calendrier-individuel-de-soutenance.xlsx
+++ b/Soutenance/calendrier-individuel-de-soutenance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Desktop\These\Soutenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Desktop\These\Thesis\Soutenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Calendrier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -412,6 +412,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -472,17 +483,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2795,8 +2795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2808,27 +2808,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
@@ -2836,37 +2836,37 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
     </row>
     <row r="5" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
@@ -2874,11 +2874,11 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10"/>
@@ -2890,7 +2890,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="3">
         <f ca="1">TODAY()</f>
-        <v>42913</v>
+        <v>42984</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -2908,30 +2908,30 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I12" s="3"/>
@@ -2974,26 +2974,26 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:14" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G17" s="34" t="s">
+      <c r="G17" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="34"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="25">
+      <c r="F18" s="25"/>
+      <c r="G18" s="28">
         <v>43089</v>
       </c>
-      <c r="H18" s="26"/>
+      <c r="H18" s="29"/>
     </row>
     <row r="19" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
@@ -3102,14 +3102,14 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="13">
+      <c r="G27" s="16">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-98,G18-70)))</f>
         <v>43019</v>
       </c>
       <c r="H27" s="6"/>
-      <c r="I27" s="16" t="str">
+      <c r="I27" s="19" t="str">
         <f ca="1">IF(G18="","",(IF(G27&lt;I8,"Hors délais (retard : "&amp;I8-G27&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G27-I8)&amp;""))</f>
-        <v>Dans les délais : J-106</v>
+        <v>Dans les délais : J-35</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -3124,9 +3124,9 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="14"/>
+      <c r="G28" s="17"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="17"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -3140,9 +3140,9 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="15"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="18"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -3204,14 +3204,14 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="13">
+      <c r="G33" s="16">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-91,G18-63)))</f>
         <v>43026</v>
       </c>
       <c r="H33" s="6"/>
-      <c r="I33" s="16" t="str">
+      <c r="I33" s="19" t="str">
         <f ca="1">IF(G18="","",(IF(G33&lt;I8,"Hors délais (retard : "&amp;I8-G33&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G33-I8)&amp;""))</f>
-        <v>Dans les délais : J-113</v>
+        <v>Dans les délais : J-42</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -3226,9 +3226,9 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="14"/>
+      <c r="G34" s="17"/>
       <c r="H34" s="6"/>
-      <c r="I34" s="17"/>
+      <c r="I34" s="20"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -3242,9 +3242,9 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="15"/>
+      <c r="G35" s="18"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="18"/>
+      <c r="I35" s="21"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -3306,14 +3306,14 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="13">
+      <c r="G39" s="16">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-84,G18-56)))</f>
         <v>43033</v>
       </c>
       <c r="H39" s="6"/>
-      <c r="I39" s="16" t="str">
+      <c r="I39" s="19" t="str">
         <f ca="1">IF(G18="","",(IF(G39&lt;I8,"Hors délais (retard : "&amp;I8-G39&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G39-I8)&amp;""))</f>
-        <v>Dans les délais : J-120</v>
+        <v>Dans les délais : J-49</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3328,9 +3328,9 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="14"/>
+      <c r="G40" s="17"/>
       <c r="H40" s="6"/>
-      <c r="I40" s="17"/>
+      <c r="I40" s="20"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
@@ -3344,9 +3344,9 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="14"/>
+      <c r="G41" s="17"/>
       <c r="H41" s="6"/>
-      <c r="I41" s="17"/>
+      <c r="I41" s="20"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
@@ -3360,9 +3360,9 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="14"/>
+      <c r="G42" s="17"/>
       <c r="H42" s="6"/>
-      <c r="I42" s="17"/>
+      <c r="I42" s="20"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
@@ -3376,9 +3376,9 @@
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="14"/>
+      <c r="G43" s="17"/>
       <c r="H43" s="6"/>
-      <c r="I43" s="17"/>
+      <c r="I43" s="20"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
@@ -3392,9 +3392,9 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="14"/>
+      <c r="G44" s="17"/>
       <c r="H44" s="6"/>
-      <c r="I44" s="17"/>
+      <c r="I44" s="20"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
@@ -3408,9 +3408,9 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="14"/>
+      <c r="G45" s="17"/>
       <c r="H45" s="6"/>
-      <c r="I45" s="17"/>
+      <c r="I45" s="20"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
@@ -3424,9 +3424,9 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="14"/>
+      <c r="G46" s="17"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="17"/>
+      <c r="I46" s="20"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
@@ -3440,9 +3440,9 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="14"/>
+      <c r="G47" s="17"/>
       <c r="H47" s="6"/>
-      <c r="I47" s="17"/>
+      <c r="I47" s="20"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
@@ -3456,9 +3456,9 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="14"/>
+      <c r="G48" s="17"/>
       <c r="H48" s="6"/>
-      <c r="I48" s="17"/>
+      <c r="I48" s="20"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
@@ -3472,9 +3472,9 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="14"/>
+      <c r="G49" s="17"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="17"/>
+      <c r="I49" s="20"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
@@ -3488,9 +3488,9 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="15"/>
+      <c r="G50" s="18"/>
       <c r="H50" s="6"/>
-      <c r="I50" s="18"/>
+      <c r="I50" s="21"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -3552,23 +3552,23 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="13">
+      <c r="G54" s="16">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-56,G18-28)))</f>
         <v>43061</v>
       </c>
       <c r="H54" s="6"/>
-      <c r="I54" s="16" t="str">
+      <c r="I54" s="19" t="str">
         <f ca="1">IF(G18="","",(IF(G54&lt;I8,"Hors délais (retard : "&amp;I8-G54&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G54-I8)&amp;""))</f>
-        <v>Dans les délais : J-148</v>
+        <v>Dans les délais : J-77</v>
       </c>
-      <c r="J54" s="32" t="str">
+      <c r="J54" s="13" t="str">
         <f>IF(AND(G54&gt;DATEVALUE("28/07/2017"),G54&lt;DATEVALUE("21/08/2017")),"Cette échéance tombe durant la fermeture obligatoire de l'Université. Cette action sera réalisée dans les plus brefs délais à la réouverture du service le 21/08/2017","")</f>
         <v/>
       </c>
-      <c r="K54" s="33"/>
-      <c r="L54" s="33"/>
-      <c r="M54" s="33"/>
-      <c r="N54" s="33"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
@@ -3577,14 +3577,14 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="14"/>
+      <c r="G55" s="17"/>
       <c r="H55" s="6"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="33"/>
-      <c r="L55" s="33"/>
-      <c r="M55" s="33"/>
-      <c r="N55" s="33"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
     </row>
     <row r="56" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
@@ -3593,14 +3593,14 @@
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="15"/>
+      <c r="G56" s="18"/>
       <c r="H56" s="6"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="33"/>
-      <c r="L56" s="33"/>
-      <c r="M56" s="33"/>
-      <c r="N56" s="33"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="14"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
@@ -3673,23 +3673,23 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="13">
+      <c r="G61" s="16">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-49,G18-21)))</f>
         <v>43068</v>
       </c>
       <c r="H61" s="6"/>
-      <c r="I61" s="16" t="str">
+      <c r="I61" s="19" t="str">
         <f ca="1">IF(G18="","",(IF(G61&lt;I8,"Hors délais (retard : "&amp;I8-G61&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G61-I8)&amp;""))</f>
-        <v>Dans les délais : J-155</v>
+        <v>Dans les délais : J-84</v>
       </c>
-      <c r="J61" s="32" t="str">
+      <c r="J61" s="13" t="str">
         <f>IF(AND(G61&gt;DATEVALUE("28/07/2017"),G61&lt;DATEVALUE("21/08/2017")),"Cette échéance tombe durant la fermeture obligatoire de l'Université. Cette action sera réalisée dans les plus brefs délais à la réouverture du service le 21/08/2017","")</f>
         <v/>
       </c>
-      <c r="K61" s="33"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="33"/>
-      <c r="N61" s="33"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="14"/>
+      <c r="N61" s="14"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
@@ -3698,14 +3698,14 @@
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
-      <c r="G62" s="14"/>
+      <c r="G62" s="17"/>
       <c r="H62" s="6"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="32"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="33"/>
-      <c r="M62" s="33"/>
-      <c r="N62" s="33"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
     </row>
     <row r="63" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
@@ -3714,14 +3714,14 @@
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="15"/>
+      <c r="G63" s="18"/>
       <c r="H63" s="6"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="32"/>
-      <c r="K63" s="33"/>
-      <c r="L63" s="33"/>
-      <c r="M63" s="33"/>
-      <c r="N63" s="33"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
+      <c r="N63" s="14"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
@@ -3794,12 +3794,12 @@
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
-      <c r="G68" s="13">
+      <c r="G68" s="16">
         <f>IF(G18="","",G18)</f>
         <v>43089</v>
       </c>
       <c r="H68" s="6"/>
-      <c r="I68" s="16" t="s">
+      <c r="I68" s="19" t="s">
         <v>3</v>
       </c>
       <c r="J68" s="4"/>
@@ -3815,9 +3815,9 @@
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
-      <c r="G69" s="14"/>
+      <c r="G69" s="17"/>
       <c r="H69" s="6"/>
-      <c r="I69" s="17"/>
+      <c r="I69" s="20"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
@@ -3831,9 +3831,9 @@
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
-      <c r="G70" s="15"/>
+      <c r="G70" s="18"/>
       <c r="H70" s="6"/>
-      <c r="I70" s="18"/>
+      <c r="I70" s="21"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
@@ -3895,14 +3895,14 @@
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
-      <c r="G74" s="13">
+      <c r="G74" s="16">
         <f>IF(G18="","",(G18+90))</f>
         <v>43179</v>
       </c>
       <c r="H74" s="6"/>
-      <c r="I74" s="16" t="str">
+      <c r="I74" s="19" t="str">
         <f ca="1">IF(G18="","",(IF(G74&lt;I8,"Hors délais (retard : "&amp;I8-G74&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G74-I8)&amp;""))</f>
-        <v>Dans les délais : J-266</v>
+        <v>Dans les délais : J-195</v>
       </c>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
@@ -3917,9 +3917,9 @@
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="14"/>
+      <c r="G75" s="17"/>
       <c r="H75" s="6"/>
-      <c r="I75" s="17"/>
+      <c r="I75" s="20"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
@@ -3933,9 +3933,9 @@
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="15"/>
+      <c r="G76" s="18"/>
       <c r="H76" s="6"/>
-      <c r="I76" s="18"/>
+      <c r="I76" s="21"/>
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
@@ -3996,6 +3996,20 @@
     <protectedRange algorithmName="SHA-512" hashValue="cdJ+a8pPbX57dbKvZhAjKevnvuWySKFJFirWIFCKRS1M63Sa0uTfdiDWXlhAoPCq/4vMdT2KANN66djY9aWMjA==" saltValue="rwNpNAq8OE+taBy9RDCX6A==" spinCount="100000" sqref="G18" name="Plage1"/>
   </protectedRanges>
   <mergeCells count="23">
+    <mergeCell ref="G74:G76"/>
+    <mergeCell ref="I74:I76"/>
+    <mergeCell ref="I68:I70"/>
+    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="I54:I56"/>
+    <mergeCell ref="G61:G63"/>
+    <mergeCell ref="I61:I63"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="G1:K7"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:H19"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="A5:E5"/>
     <mergeCell ref="J54:N56"/>
     <mergeCell ref="J61:N63"/>
     <mergeCell ref="G17:H17"/>
@@ -4005,20 +4019,6 @@
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="G33:G35"/>
     <mergeCell ref="I33:I35"/>
-    <mergeCell ref="G1:K7"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="G18:H19"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="G74:G76"/>
-    <mergeCell ref="I74:I76"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="G54:G56"/>
-    <mergeCell ref="I54:I56"/>
-    <mergeCell ref="G61:G63"/>
-    <mergeCell ref="I61:I63"/>
-    <mergeCell ref="G68:G70"/>
   </mergeCells>
   <conditionalFormatting sqref="I27:I29">
     <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="Hors délais">

</xml_diff>

<commit_message>
change in style (chapter) + added publications and acronyms
</commit_message>
<xml_diff>
--- a/Soutenance/calendrier-individuel-de-soutenance.xlsx
+++ b/Soutenance/calendrier-individuel-de-soutenance.xlsx
@@ -412,17 +412,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -483,6 +472,17 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2795,8 +2795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2808,27 +2808,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
@@ -2836,37 +2836,37 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
     </row>
     <row r="5" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
     </row>
     <row r="6" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
@@ -2874,11 +2874,11 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10"/>
@@ -2890,7 +2890,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="3">
         <f ca="1">TODAY()</f>
-        <v>42984</v>
+        <v>43005</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -2908,30 +2908,30 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I12" s="3"/>
@@ -2974,26 +2974,26 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:14" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="15"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="28">
-        <v>43089</v>
+      <c r="F18" s="22"/>
+      <c r="G18" s="25">
+        <v>43077</v>
       </c>
-      <c r="H18" s="29"/>
+      <c r="H18" s="26"/>
     </row>
     <row r="19" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="26"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
@@ -3102,14 +3102,14 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="16">
+      <c r="G27" s="13">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-98,G18-70)))</f>
-        <v>43019</v>
+        <v>43007</v>
       </c>
       <c r="H27" s="6"/>
-      <c r="I27" s="19" t="str">
+      <c r="I27" s="16" t="str">
         <f ca="1">IF(G18="","",(IF(G27&lt;I8,"Hors délais (retard : "&amp;I8-G27&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G27-I8)&amp;""))</f>
-        <v>Dans les délais : J-35</v>
+        <v>Dans les délais : J-2</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -3124,9 +3124,9 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="14"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="20"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -3140,9 +3140,9 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="18"/>
+      <c r="G29" s="15"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="21"/>
+      <c r="I29" s="18"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -3204,14 +3204,14 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="16">
+      <c r="G33" s="13">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-91,G18-63)))</f>
-        <v>43026</v>
+        <v>43014</v>
       </c>
       <c r="H33" s="6"/>
-      <c r="I33" s="19" t="str">
+      <c r="I33" s="16" t="str">
         <f ca="1">IF(G18="","",(IF(G33&lt;I8,"Hors délais (retard : "&amp;I8-G33&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G33-I8)&amp;""))</f>
-        <v>Dans les délais : J-42</v>
+        <v>Dans les délais : J-9</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -3226,9 +3226,9 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="17"/>
+      <c r="G34" s="14"/>
       <c r="H34" s="6"/>
-      <c r="I34" s="20"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -3242,9 +3242,9 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="18"/>
+      <c r="G35" s="15"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="21"/>
+      <c r="I35" s="18"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -3306,14 +3306,14 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="16">
+      <c r="G39" s="13">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-84,G18-56)))</f>
-        <v>43033</v>
+        <v>43021</v>
       </c>
       <c r="H39" s="6"/>
-      <c r="I39" s="19" t="str">
+      <c r="I39" s="16" t="str">
         <f ca="1">IF(G18="","",(IF(G39&lt;I8,"Hors délais (retard : "&amp;I8-G39&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G39-I8)&amp;""))</f>
-        <v>Dans les délais : J-49</v>
+        <v>Dans les délais : J-16</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3328,9 +3328,9 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="17"/>
+      <c r="G40" s="14"/>
       <c r="H40" s="6"/>
-      <c r="I40" s="20"/>
+      <c r="I40" s="17"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
@@ -3344,9 +3344,9 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="17"/>
+      <c r="G41" s="14"/>
       <c r="H41" s="6"/>
-      <c r="I41" s="20"/>
+      <c r="I41" s="17"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
@@ -3360,9 +3360,9 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="17"/>
+      <c r="G42" s="14"/>
       <c r="H42" s="6"/>
-      <c r="I42" s="20"/>
+      <c r="I42" s="17"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
@@ -3376,9 +3376,9 @@
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="17"/>
+      <c r="G43" s="14"/>
       <c r="H43" s="6"/>
-      <c r="I43" s="20"/>
+      <c r="I43" s="17"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
@@ -3392,9 +3392,9 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="17"/>
+      <c r="G44" s="14"/>
       <c r="H44" s="6"/>
-      <c r="I44" s="20"/>
+      <c r="I44" s="17"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
@@ -3408,9 +3408,9 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="17"/>
+      <c r="G45" s="14"/>
       <c r="H45" s="6"/>
-      <c r="I45" s="20"/>
+      <c r="I45" s="17"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
@@ -3424,9 +3424,9 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="17"/>
+      <c r="G46" s="14"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="20"/>
+      <c r="I46" s="17"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
@@ -3440,9 +3440,9 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="17"/>
+      <c r="G47" s="14"/>
       <c r="H47" s="6"/>
-      <c r="I47" s="20"/>
+      <c r="I47" s="17"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
@@ -3456,9 +3456,9 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="17"/>
+      <c r="G48" s="14"/>
       <c r="H48" s="6"/>
-      <c r="I48" s="20"/>
+      <c r="I48" s="17"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
@@ -3472,9 +3472,9 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="17"/>
+      <c r="G49" s="14"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="20"/>
+      <c r="I49" s="17"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
@@ -3488,9 +3488,9 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="18"/>
+      <c r="G50" s="15"/>
       <c r="H50" s="6"/>
-      <c r="I50" s="21"/>
+      <c r="I50" s="18"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -3552,23 +3552,23 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="16">
+      <c r="G54" s="13">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-56,G18-28)))</f>
-        <v>43061</v>
+        <v>43049</v>
       </c>
       <c r="H54" s="6"/>
-      <c r="I54" s="19" t="str">
+      <c r="I54" s="16" t="str">
         <f ca="1">IF(G18="","",(IF(G54&lt;I8,"Hors délais (retard : "&amp;I8-G54&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G54-I8)&amp;""))</f>
-        <v>Dans les délais : J-77</v>
+        <v>Dans les délais : J-44</v>
       </c>
-      <c r="J54" s="13" t="str">
+      <c r="J54" s="32" t="str">
         <f>IF(AND(G54&gt;DATEVALUE("28/07/2017"),G54&lt;DATEVALUE("21/08/2017")),"Cette échéance tombe durant la fermeture obligatoire de l'Université. Cette action sera réalisée dans les plus brefs délais à la réouverture du service le 21/08/2017","")</f>
         <v/>
       </c>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
+      <c r="K54" s="33"/>
+      <c r="L54" s="33"/>
+      <c r="M54" s="33"/>
+      <c r="N54" s="33"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
@@ -3577,14 +3577,14 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="17"/>
+      <c r="G55" s="14"/>
       <c r="H55" s="6"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="33"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
+      <c r="N55" s="33"/>
     </row>
     <row r="56" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
@@ -3593,14 +3593,14 @@
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="18"/>
+      <c r="G56" s="15"/>
       <c r="H56" s="6"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+      <c r="N56" s="33"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
@@ -3673,23 +3673,23 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="16">
+      <c r="G61" s="13">
         <f>IF(G18="","",(IF(AND(G18&gt;DATEVALUE("31/08/2017"),G18&lt;DATEVALUE("16/10/2017")),G18-49,G18-21)))</f>
-        <v>43068</v>
+        <v>43056</v>
       </c>
       <c r="H61" s="6"/>
-      <c r="I61" s="19" t="str">
+      <c r="I61" s="16" t="str">
         <f ca="1">IF(G18="","",(IF(G61&lt;I8,"Hors délais (retard : "&amp;I8-G61&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G61-I8)&amp;""))</f>
-        <v>Dans les délais : J-84</v>
+        <v>Dans les délais : J-51</v>
       </c>
-      <c r="J61" s="13" t="str">
+      <c r="J61" s="32" t="str">
         <f>IF(AND(G61&gt;DATEVALUE("28/07/2017"),G61&lt;DATEVALUE("21/08/2017")),"Cette échéance tombe durant la fermeture obligatoire de l'Université. Cette action sera réalisée dans les plus brefs délais à la réouverture du service le 21/08/2017","")</f>
         <v/>
       </c>
-      <c r="K61" s="14"/>
-      <c r="L61" s="14"/>
-      <c r="M61" s="14"/>
-      <c r="N61" s="14"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="33"/>
+      <c r="N61" s="33"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
@@ -3698,14 +3698,14 @@
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
-      <c r="G62" s="17"/>
+      <c r="G62" s="14"/>
       <c r="H62" s="6"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="14"/>
-      <c r="N62" s="14"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="32"/>
+      <c r="K62" s="33"/>
+      <c r="L62" s="33"/>
+      <c r="M62" s="33"/>
+      <c r="N62" s="33"/>
     </row>
     <row r="63" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
@@ -3714,14 +3714,14 @@
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="18"/>
+      <c r="G63" s="15"/>
       <c r="H63" s="6"/>
-      <c r="I63" s="21"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="14"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="33"/>
+      <c r="L63" s="33"/>
+      <c r="M63" s="33"/>
+      <c r="N63" s="33"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
@@ -3794,12 +3794,12 @@
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
-      <c r="G68" s="16">
+      <c r="G68" s="13">
         <f>IF(G18="","",G18)</f>
-        <v>43089</v>
+        <v>43077</v>
       </c>
       <c r="H68" s="6"/>
-      <c r="I68" s="19" t="s">
+      <c r="I68" s="16" t="s">
         <v>3</v>
       </c>
       <c r="J68" s="4"/>
@@ -3815,9 +3815,9 @@
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
-      <c r="G69" s="17"/>
+      <c r="G69" s="14"/>
       <c r="H69" s="6"/>
-      <c r="I69" s="20"/>
+      <c r="I69" s="17"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
@@ -3831,9 +3831,9 @@
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
-      <c r="G70" s="18"/>
+      <c r="G70" s="15"/>
       <c r="H70" s="6"/>
-      <c r="I70" s="21"/>
+      <c r="I70" s="18"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
@@ -3895,14 +3895,14 @@
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
-      <c r="G74" s="16">
+      <c r="G74" s="13">
         <f>IF(G18="","",(G18+90))</f>
-        <v>43179</v>
+        <v>43167</v>
       </c>
       <c r="H74" s="6"/>
-      <c r="I74" s="19" t="str">
+      <c r="I74" s="16" t="str">
         <f ca="1">IF(G18="","",(IF(G74&lt;I8,"Hors délais (retard : "&amp;I8-G74&amp;" "&amp;"jours)","Dans les délais"&amp;" "&amp;": J-"&amp;G74-I8)&amp;""))</f>
-        <v>Dans les délais : J-195</v>
+        <v>Dans les délais : J-162</v>
       </c>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
@@ -3917,9 +3917,9 @@
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="17"/>
+      <c r="G75" s="14"/>
       <c r="H75" s="6"/>
-      <c r="I75" s="20"/>
+      <c r="I75" s="17"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
@@ -3933,9 +3933,9 @@
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="18"/>
+      <c r="G76" s="15"/>
       <c r="H76" s="6"/>
-      <c r="I76" s="21"/>
+      <c r="I76" s="18"/>
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
@@ -3996,20 +3996,6 @@
     <protectedRange algorithmName="SHA-512" hashValue="cdJ+a8pPbX57dbKvZhAjKevnvuWySKFJFirWIFCKRS1M63Sa0uTfdiDWXlhAoPCq/4vMdT2KANN66djY9aWMjA==" saltValue="rwNpNAq8OE+taBy9RDCX6A==" spinCount="100000" sqref="G18" name="Plage1"/>
   </protectedRanges>
   <mergeCells count="23">
-    <mergeCell ref="G74:G76"/>
-    <mergeCell ref="I74:I76"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="G54:G56"/>
-    <mergeCell ref="I54:I56"/>
-    <mergeCell ref="G61:G63"/>
-    <mergeCell ref="I61:I63"/>
-    <mergeCell ref="G68:G70"/>
-    <mergeCell ref="G1:K7"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="G18:H19"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="A5:E5"/>
     <mergeCell ref="J54:N56"/>
     <mergeCell ref="J61:N63"/>
     <mergeCell ref="G17:H17"/>
@@ -4019,6 +4005,20 @@
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="G33:G35"/>
     <mergeCell ref="I33:I35"/>
+    <mergeCell ref="G1:K7"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:H19"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="G74:G76"/>
+    <mergeCell ref="I74:I76"/>
+    <mergeCell ref="I68:I70"/>
+    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="I54:I56"/>
+    <mergeCell ref="G61:G63"/>
+    <mergeCell ref="I61:I63"/>
+    <mergeCell ref="G68:G70"/>
   </mergeCells>
   <conditionalFormatting sqref="I27:I29">
     <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="Hors délais">

</xml_diff>